<commit_message>
Changes to XL file
</commit_message>
<xml_diff>
--- a/Contract.xlsx
+++ b/Contract.xlsx
@@ -13,10 +13,10 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1582747315" val="974" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1582747315" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1582747315" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1582747315"/>
+      <pm:revision xmlns:pm="smNativeData" day="1582902452" val="974" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1582902452" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1582902452" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1582902452"/>
     </ext>
   </extLst>
 </workbook>
@@ -67,7 +67,7 @@
     <t>IPFS Infura Gateway</t>
   </si>
   <si>
-    <t>https://ipfs.infura.io:5001/api/v0/block/get?arg=&lt;key&gt;</t>
+    <t>https://ipfs.infura.io:5001/api/v0/block/get?arg=QmQv9RDA4LPLsQzFUncHmtw8kWWJBrnqyxQm53marjXPFY</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1582747315" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1582902452" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -107,7 +107,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1582747315" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1582902452" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -123,7 +123,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1582747315" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1582902452" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -145,7 +145,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1582747315" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1582902452" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -167,7 +167,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1582747315"/>
+          <pm:border xmlns:pm="smNativeData" id="1582902452"/>
         </ext>
       </extLst>
     </border>
@@ -186,7 +186,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1582747315"/>
+          <pm:border xmlns:pm="smNativeData" id="1582902452"/>
         </ext>
       </extLst>
     </border>
@@ -209,7 +209,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1582747315" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1582902452" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -553,7 +553,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1582747315" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1582902452" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -562,14 +562,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1582747315" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1582747315" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1582902452" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1582902452" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1582747315" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1582902452" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>